<commit_message>
update BOM to own parts
Added own prices from Aliexpress, for part sourced from Aliexpress.
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_2.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Johansson\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Mój dysk\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D15EB-E14F-4425-B457-83219F0BB8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698097E8-FED4-49A1-BFC7-D9D94508F348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="259">
   <si>
     <t>References</t>
   </si>
@@ -785,6 +785,25 @@
   </si>
   <si>
     <t>AxxSolder V3.2</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Wydatki w sumie</t>
+  </si>
+  <si>
+    <t>za szt.</t>
+  </si>
+  <si>
+    <t>na ile urządzeń</t>
+  </si>
+  <si>
+    <t>Ilość zamówiona Aliexpress</t>
+  </si>
+  <si>
+    <t>koszt /
+1 urządzenie</t>
   </si>
 </sst>
 </file>
@@ -792,17 +811,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -828,12 +855,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
@@ -849,8 +870,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -887,8 +942,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -935,67 +996,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1003,10 +1115,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1020,9 +1140,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1060,7 +1180,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1166,7 +1286,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1317,47 +1437,51 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ACC24B-AB82-4A13-8EC7-565525F2C562}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="19" customWidth="1"/>
+    <col min="12" max="12" width="13" style="19" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="19"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="35" t="s">
         <v>207</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>238</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="21"/>
-      <c r="B2" s="23"/>
+    <row r="2" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="4" t="s">
         <v>237</v>
       </c>
@@ -1369,39 +1493,54 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>155</v>
       </c>
@@ -1423,53 +1562,89 @@
       <c r="G4" s="1">
         <v>17</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <f>G4*H4</f>
         <v>0.73099999999999998</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="17">
         <f>1.25*I4</f>
         <v>0.91374999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="K4" s="20">
+        <v>100</v>
+      </c>
+      <c r="L4" s="27">
+        <v>2.73</v>
+      </c>
+      <c r="M4" s="22">
+        <f>IF(K4&gt;0,L4/K4,"")</f>
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="N4" s="20">
+        <f t="shared" ref="N4:N47" si="0">IF(K4&gt;0,K4/G4,"")</f>
+        <v>5.882352941176471</v>
+      </c>
+      <c r="O4" s="16">
+        <f>G4*M4</f>
+        <v>0.46410000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>16</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I5" s="13">
-        <f t="shared" ref="I5:I47" si="0">G5*H5</f>
+      <c r="I5" s="11">
+        <f t="shared" ref="I5:I47" si="1">G5*H5</f>
         <v>2.8319999999999999</v>
       </c>
-      <c r="J5" s="13">
-        <f t="shared" ref="J5:J47" si="1">1.25*I5</f>
+      <c r="J5" s="17">
+        <f t="shared" ref="J5:J47" si="2">1.25*I5</f>
         <v>3.54</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="20">
+        <v>50</v>
+      </c>
+      <c r="L5" s="22">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M5" s="22">
+        <f t="shared" ref="M5:M45" si="3">IF(K5&gt;0,L5/K5,"")</f>
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="N5" s="20">
+        <f t="shared" si="0"/>
+        <v>3.125</v>
+      </c>
+      <c r="O5" s="16">
+        <f t="shared" ref="O5:O44" si="4">G5*M5</f>
+        <v>5.4720000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>157</v>
       </c>
@@ -1491,57 +1666,93 @@
       <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.186</v>
+      </c>
+      <c r="J6" s="17">
+        <f t="shared" si="2"/>
+        <v>0.23249999999999998</v>
+      </c>
+      <c r="K6" s="20">
+        <v>100</v>
+      </c>
+      <c r="L6" s="22">
+        <v>2.73</v>
+      </c>
+      <c r="M6" s="22">
+        <f t="shared" si="3"/>
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="N6" s="20">
         <f t="shared" si="0"/>
-        <v>0.186</v>
-      </c>
-      <c r="J6" s="13">
+        <v>50</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="4"/>
+        <v>5.4600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="I7" s="11">
         <f t="shared" si="1"/>
-        <v>0.23249999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14">
         <v>0.61399999999999999</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="17">
+        <f t="shared" si="2"/>
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="K7" s="20">
+        <v>10</v>
+      </c>
+      <c r="L7" s="22">
+        <v>11.02</v>
+      </c>
+      <c r="M7" s="22">
+        <f t="shared" si="3"/>
+        <v>1.1019999999999999</v>
+      </c>
+      <c r="N7" s="20">
         <f t="shared" si="0"/>
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="J7" s="13">
-        <f t="shared" si="1"/>
-        <v>0.76749999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O7" s="16">
+        <f t="shared" si="4"/>
+        <v>1.1019999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1559,57 +1770,93 @@
       <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="11">
         <v>0.125</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="J8" s="17">
+        <f t="shared" si="2"/>
+        <v>3.125</v>
+      </c>
+      <c r="K8" s="20">
+        <v>100</v>
+      </c>
+      <c r="L8" s="22">
+        <v>1</v>
+      </c>
+      <c r="M8" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N8" s="20">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="J8" s="13">
+        <v>5</v>
+      </c>
+      <c r="O8" s="16">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="10">
+        <v>5</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I9" s="11">
         <f t="shared" si="1"/>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="11" t="s">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="J9" s="17">
+        <f t="shared" si="2"/>
+        <v>0.87500000000000011</v>
+      </c>
+      <c r="K9" s="20">
+        <v>100</v>
+      </c>
+      <c r="L9" s="22">
+        <v>1</v>
+      </c>
+      <c r="M9" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N9" s="20">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="11">
-        <v>5</v>
-      </c>
-      <c r="H9" s="14">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I9" s="13">
-        <f t="shared" si="0"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="J9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.87500000000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O9" s="16">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1627,57 +1874,93 @@
       <c r="G10" s="1">
         <v>4</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>0.214</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="11">
+        <f t="shared" si="1"/>
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="J10" s="17">
+        <f t="shared" si="2"/>
+        <v>1.07</v>
+      </c>
+      <c r="K10" s="20">
+        <v>100</v>
+      </c>
+      <c r="L10" s="22">
+        <v>1</v>
+      </c>
+      <c r="M10" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N10" s="20">
         <f t="shared" si="0"/>
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="J10" s="13">
+        <v>25</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" si="4"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="10">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.121</v>
+      </c>
+      <c r="I11" s="11">
         <f t="shared" si="1"/>
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="11">
-        <v>4</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0.121</v>
-      </c>
-      <c r="I11" s="13">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="2"/>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="K11" s="20">
+        <v>100</v>
+      </c>
+      <c r="L11" s="22">
+        <v>1</v>
+      </c>
+      <c r="M11" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N11" s="20">
         <f t="shared" si="0"/>
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="J11" s="13">
-        <f t="shared" si="1"/>
-        <v>0.60499999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="O11" s="16">
+        <f t="shared" si="4"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="18" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1695,57 +1978,93 @@
       <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <v>0.121</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
+        <f t="shared" si="1"/>
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="2"/>
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="K12" s="20">
+        <v>100</v>
+      </c>
+      <c r="L12" s="22">
+        <v>1</v>
+      </c>
+      <c r="M12" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N12" s="20">
         <f t="shared" si="0"/>
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="J12" s="13">
+        <v>50</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="4"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="18">
+        <v>100</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="10">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0.307</v>
+      </c>
+      <c r="I13" s="11">
         <f t="shared" si="1"/>
-        <v>0.30249999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="B13" s="11">
+        <v>2.149</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" si="2"/>
+        <v>2.6862500000000002</v>
+      </c>
+      <c r="K13" s="20">
         <v>100</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="11">
-        <v>7</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0.307</v>
-      </c>
-      <c r="I13" s="13">
+      <c r="L13" s="22">
+        <v>1</v>
+      </c>
+      <c r="M13" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N13" s="20">
         <f t="shared" si="0"/>
-        <v>2.149</v>
-      </c>
-      <c r="J13" s="13">
-        <f t="shared" si="1"/>
-        <v>2.6862500000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14.285714285714286</v>
+      </c>
+      <c r="O13" s="16">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1763,57 +2082,93 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <v>0.753</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
+        <f t="shared" si="1"/>
+        <v>0.753</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="2"/>
+        <v>0.94125000000000003</v>
+      </c>
+      <c r="K14" s="20">
+        <v>50</v>
+      </c>
+      <c r="L14" s="22">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M14" s="22">
+        <f t="shared" si="3"/>
+        <v>0.16399999999999998</v>
+      </c>
+      <c r="N14" s="20">
         <f t="shared" si="0"/>
-        <v>0.753</v>
-      </c>
-      <c r="J14" s="13">
+        <v>50</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="4"/>
+        <v>0.16399999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I15" s="11">
         <f t="shared" si="1"/>
-        <v>0.94125000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="14">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I15" s="13">
+      <c r="J15" s="17">
+        <f t="shared" si="2"/>
+        <v>0.11624999999999999</v>
+      </c>
+      <c r="K15" s="20">
+        <v>100</v>
+      </c>
+      <c r="L15" s="22">
+        <v>0</v>
+      </c>
+      <c r="M15" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="20">
         <f t="shared" si="0"/>
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="J15" s="13">
-        <f t="shared" si="1"/>
-        <v>0.11624999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="18" t="s">
         <v>217</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1831,26 +2186,44 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="11">
         <v>0.40899999999999997</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="11">
+        <f t="shared" si="1"/>
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="2"/>
+        <v>0.51124999999999998</v>
+      </c>
+      <c r="K16" s="20">
+        <v>100</v>
+      </c>
+      <c r="L16" s="22">
+        <v>5.7</v>
+      </c>
+      <c r="M16" s="22">
+        <f t="shared" si="3"/>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="N16" s="20">
         <f t="shared" si="0"/>
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="J16" s="13">
-        <f t="shared" si="1"/>
-        <v>0.51124999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="4"/>
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="18">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1865,53 +2238,89 @@
       <c r="G17" s="1">
         <v>2</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="12">
         <v>0.121</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="2"/>
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="K17" s="20">
+        <v>100</v>
+      </c>
+      <c r="L17" s="22">
+        <v>1</v>
+      </c>
+      <c r="M17" s="22">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="N17" s="20">
         <f t="shared" si="0"/>
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="J17" s="13">
+        <v>50</v>
+      </c>
+      <c r="O17" s="16">
+        <f t="shared" si="4"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.753</v>
+      </c>
+      <c r="I18" s="11">
         <f t="shared" si="1"/>
-        <v>0.30249999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="G18" s="11">
-        <v>1</v>
-      </c>
-      <c r="H18" s="14">
         <v>0.753</v>
       </c>
-      <c r="I18" s="13">
+      <c r="J18" s="17">
+        <f t="shared" si="2"/>
+        <v>0.94125000000000003</v>
+      </c>
+      <c r="K18" s="20">
+        <v>20</v>
+      </c>
+      <c r="L18" s="22">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M18" s="22">
+        <f t="shared" si="3"/>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="N18" s="20">
         <f t="shared" si="0"/>
-        <v>0.753</v>
-      </c>
-      <c r="J18" s="13">
-        <f t="shared" si="1"/>
-        <v>0.94125000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="O18" s="16">
+        <f t="shared" si="4"/>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -1933,55 +2342,89 @@
       <c r="G19" s="1">
         <v>4</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="11">
         <v>0.112</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="11">
+        <f t="shared" si="1"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" si="2"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K19" s="20">
+        <v>50</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0</v>
+      </c>
+      <c r="M19" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="20">
         <f t="shared" si="0"/>
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="J19" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="O19" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I20" s="11">
         <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="11" t="s">
+        <v>0.39</v>
+      </c>
+      <c r="J20" s="17">
+        <f t="shared" si="2"/>
+        <v>0.48750000000000004</v>
+      </c>
+      <c r="K20" s="21">
+        <v>100</v>
+      </c>
+      <c r="L20" s="22">
+        <v>21.5</v>
+      </c>
+      <c r="M20" s="22">
+        <f t="shared" si="3"/>
+        <v>0.215</v>
+      </c>
+      <c r="N20" s="20">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="11">
-        <v>2</v>
-      </c>
-      <c r="H20" s="14">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="I20" s="13">
-        <f t="shared" si="0"/>
-        <v>0.39</v>
-      </c>
-      <c r="J20" s="13">
-        <f t="shared" si="1"/>
-        <v>0.48750000000000004</v>
-      </c>
-      <c r="K20" s="12"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O20" s="16">
+        <f t="shared" si="4"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -2003,55 +2446,89 @@
       <c r="G21" s="1">
         <v>2</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="11">
         <v>0.4</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="28">
+        <v>50</v>
+      </c>
+      <c r="L21" s="22">
+        <v>9</v>
+      </c>
+      <c r="M21" s="22">
+        <f t="shared" si="3"/>
+        <v>0.18</v>
+      </c>
+      <c r="N21" s="20">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J21" s="13">
+        <v>25</v>
+      </c>
+      <c r="O21" s="16">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="10">
+        <v>2</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0.372</v>
+      </c>
+      <c r="I22" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K21" s="12"/>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="11">
-        <v>2</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0.372</v>
-      </c>
-      <c r="I22" s="13">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J22" s="17">
+        <f t="shared" si="2"/>
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="K22" s="20">
+        <v>100</v>
+      </c>
+      <c r="L22" s="22">
+        <v>32</v>
+      </c>
+      <c r="M22" s="22">
+        <f t="shared" si="3"/>
+        <v>0.32</v>
+      </c>
+      <c r="N22" s="20">
         <f t="shared" si="0"/>
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="J22" s="13">
-        <f t="shared" si="1"/>
-        <v>0.92999999999999994</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="O22" s="16">
+        <f t="shared" si="4"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>242</v>
       </c>
@@ -2073,53 +2550,89 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="11">
         <v>18.55</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
+        <f t="shared" si="1"/>
+        <v>18.55</v>
+      </c>
+      <c r="J23" s="17">
+        <f t="shared" si="2"/>
+        <v>23.1875</v>
+      </c>
+      <c r="K23" s="20">
+        <v>2</v>
+      </c>
+      <c r="L23" s="22">
+        <v>36</v>
+      </c>
+      <c r="M23" s="22">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="N23" s="20">
         <f t="shared" si="0"/>
-        <v>18.55</v>
-      </c>
-      <c r="J23" s="13">
+        <v>2</v>
+      </c>
+      <c r="O23" s="16">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="10">
+        <v>1</v>
+      </c>
+      <c r="H24" s="12">
+        <v>2.37</v>
+      </c>
+      <c r="I24" s="11">
         <f t="shared" si="1"/>
-        <v>23.1875</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G24" s="11">
-        <v>1</v>
-      </c>
-      <c r="H24" s="14">
         <v>2.37</v>
       </c>
-      <c r="I24" s="13">
+      <c r="J24" s="17">
+        <f t="shared" si="2"/>
+        <v>2.9625000000000004</v>
+      </c>
+      <c r="K24" s="20">
+        <v>5</v>
+      </c>
+      <c r="L24" s="22">
+        <v>16</v>
+      </c>
+      <c r="M24" s="22">
+        <f t="shared" si="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="N24" s="20">
         <f t="shared" si="0"/>
-        <v>2.37</v>
-      </c>
-      <c r="J24" s="13">
-        <f t="shared" si="1"/>
-        <v>2.9625000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="O24" s="16">
+        <f t="shared" si="4"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2141,53 +2654,89 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="11">
         <v>1.6</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="J25" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K25" s="20">
+        <v>5</v>
+      </c>
+      <c r="L25" s="22">
+        <v>21.5</v>
+      </c>
+      <c r="M25" s="22">
+        <f t="shared" si="3"/>
+        <v>4.3</v>
+      </c>
+      <c r="N25" s="20">
         <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="J25" s="13">
+        <v>5</v>
+      </c>
+      <c r="O25" s="16">
+        <f t="shared" si="4"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+      <c r="H26" s="12">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="I26" s="11">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G26" s="11">
-        <v>1</v>
-      </c>
-      <c r="H26" s="14">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I26" s="13">
+      <c r="J26" s="17">
+        <f t="shared" si="2"/>
+        <v>3.1875</v>
+      </c>
+      <c r="K26" s="20">
+        <v>50</v>
+      </c>
+      <c r="L26" s="22">
+        <v>30</v>
+      </c>
+      <c r="M26" s="22">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="N26" s="20">
         <f t="shared" si="0"/>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="J26" s="13">
-        <f t="shared" si="1"/>
-        <v>3.1875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="O26" s="16">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -2209,53 +2758,87 @@
       <c r="G27" s="1">
         <v>1</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <v>0.72499999999999998</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="11">
+        <f t="shared" si="1"/>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="J27" s="17">
+        <f t="shared" si="2"/>
+        <v>0.90625</v>
+      </c>
+      <c r="K27" s="20">
+        <v>10</v>
+      </c>
+      <c r="L27" s="22">
+        <v>11</v>
+      </c>
+      <c r="M27" s="22">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N27" s="20">
         <f t="shared" si="0"/>
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="J27" s="13">
+        <v>10</v>
+      </c>
+      <c r="O27" s="16">
+        <f t="shared" si="4"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" s="10">
+        <v>2</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I28" s="11">
         <f t="shared" si="1"/>
-        <v>0.90625</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" s="11">
-        <v>2</v>
-      </c>
-      <c r="H28" s="14">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="I28" s="13">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="J28" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="K28" s="20">
+        <v>0</v>
+      </c>
+      <c r="L28" s="22">
+        <v>0</v>
+      </c>
+      <c r="M28" s="22">
+        <v>0</v>
+      </c>
+      <c r="N28" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>1.0980000000000001</v>
-      </c>
-      <c r="J28" s="13">
-        <f t="shared" si="1"/>
-        <v>1.3725000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2277,57 +2860,93 @@
       <c r="G29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="11">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="11">
+        <f t="shared" si="1"/>
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" si="2"/>
+        <v>0.22125</v>
+      </c>
+      <c r="K29" s="20">
+        <v>20</v>
+      </c>
+      <c r="L29" s="22">
+        <v>17.55</v>
+      </c>
+      <c r="M29" s="22">
+        <f t="shared" si="3"/>
+        <v>0.87750000000000006</v>
+      </c>
+      <c r="N29" s="20">
         <f t="shared" si="0"/>
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="J29" s="13">
+        <v>20</v>
+      </c>
+      <c r="O29" s="16">
+        <f t="shared" si="4"/>
+        <v>0.87750000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="10">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="I30" s="11">
         <f t="shared" si="1"/>
-        <v>0.22125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="G30" s="11">
-        <v>1</v>
-      </c>
-      <c r="H30" s="14">
         <v>0.38100000000000001</v>
       </c>
-      <c r="I30" s="13">
+      <c r="J30" s="17">
+        <f t="shared" si="2"/>
+        <v>0.47625000000000001</v>
+      </c>
+      <c r="K30" s="20">
+        <v>10</v>
+      </c>
+      <c r="L30" s="22">
+        <v>6.2</v>
+      </c>
+      <c r="M30" s="22">
+        <f t="shared" si="3"/>
+        <v>0.62</v>
+      </c>
+      <c r="N30" s="20">
         <f t="shared" si="0"/>
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="J30" s="13">
-        <f t="shared" si="1"/>
-        <v>0.47625000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O30" s="16">
+        <f t="shared" si="4"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -2345,57 +2964,93 @@
       <c r="G31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="11">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I31" s="13">
+      <c r="I31" s="11">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J31" s="17">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+      <c r="K31" s="20">
+        <v>10</v>
+      </c>
+      <c r="L31" s="22">
+        <v>89</v>
+      </c>
+      <c r="M31" s="22">
+        <f t="shared" si="3"/>
+        <v>8.9</v>
+      </c>
+      <c r="N31" s="20">
         <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J31" s="13">
+        <v>10</v>
+      </c>
+      <c r="O31" s="16">
+        <f t="shared" si="4"/>
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="I32" s="11">
         <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="G32" s="11">
-        <v>1</v>
-      </c>
-      <c r="H32" s="14">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I32" s="13">
+      <c r="J32" s="17">
+        <f t="shared" si="2"/>
+        <v>1.20875</v>
+      </c>
+      <c r="K32" s="20">
+        <v>10</v>
+      </c>
+      <c r="L32" s="22">
+        <v>18</v>
+      </c>
+      <c r="M32" s="22">
+        <f t="shared" si="3"/>
+        <v>1.8</v>
+      </c>
+      <c r="N32" s="20">
         <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J32" s="13">
-        <f t="shared" si="1"/>
-        <v>1.20875</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O32" s="16">
+        <f t="shared" si="4"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="18" t="s">
         <v>106</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -2413,53 +3068,89 @@
       <c r="G33" s="1">
         <v>1</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="11">
         <v>5.65</v>
       </c>
-      <c r="I33" s="13">
+      <c r="I33" s="11">
+        <f t="shared" si="1"/>
+        <v>5.65</v>
+      </c>
+      <c r="J33" s="17">
+        <f t="shared" si="2"/>
+        <v>7.0625</v>
+      </c>
+      <c r="K33" s="20">
+        <v>5</v>
+      </c>
+      <c r="L33" s="22">
+        <v>82</v>
+      </c>
+      <c r="M33" s="22">
+        <f t="shared" si="3"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="N33" s="20">
         <f t="shared" si="0"/>
-        <v>5.65</v>
-      </c>
-      <c r="J33" s="13">
+        <v>5</v>
+      </c>
+      <c r="O33" s="16">
+        <f t="shared" si="4"/>
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="I34" s="11">
         <f t="shared" si="1"/>
-        <v>7.0625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G34" s="11">
-        <v>1</v>
-      </c>
-      <c r="H34" s="14">
         <v>0.32600000000000001</v>
       </c>
-      <c r="I34" s="13">
+      <c r="J34" s="17">
+        <f t="shared" si="2"/>
+        <v>0.40750000000000003</v>
+      </c>
+      <c r="K34" s="20">
+        <v>10</v>
+      </c>
+      <c r="L34" s="22">
+        <v>8</v>
+      </c>
+      <c r="M34" s="22">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N34" s="20">
         <f t="shared" si="0"/>
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="J34" s="13">
-        <f t="shared" si="1"/>
-        <v>0.40750000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O34" s="16">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
@@ -2481,53 +3172,89 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H35" s="11">
         <v>2.52</v>
       </c>
-      <c r="I35" s="13">
+      <c r="I35" s="11">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="J35" s="17">
+        <f t="shared" si="2"/>
+        <v>3.15</v>
+      </c>
+      <c r="K35" s="20">
+        <v>5</v>
+      </c>
+      <c r="L35" s="22">
+        <v>31</v>
+      </c>
+      <c r="M35" s="22">
+        <f t="shared" si="3"/>
+        <v>6.2</v>
+      </c>
+      <c r="N35" s="20">
         <f t="shared" si="0"/>
-        <v>2.52</v>
-      </c>
-      <c r="J35" s="13">
+        <v>5</v>
+      </c>
+      <c r="O35" s="16">
+        <f t="shared" si="4"/>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1</v>
+      </c>
+      <c r="H36" s="12">
+        <v>2.64</v>
+      </c>
+      <c r="I36" s="11">
         <f t="shared" si="1"/>
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="11">
-        <v>1</v>
-      </c>
-      <c r="H36" s="14">
         <v>2.64</v>
       </c>
-      <c r="I36" s="13">
+      <c r="J36" s="17">
+        <f t="shared" si="2"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="K36" s="20">
+        <v>5</v>
+      </c>
+      <c r="L36" s="22">
+        <v>63</v>
+      </c>
+      <c r="M36" s="22">
+        <f t="shared" si="3"/>
+        <v>12.6</v>
+      </c>
+      <c r="N36" s="20">
         <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="J36" s="13">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="O36" s="16">
+        <f t="shared" si="4"/>
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>179</v>
       </c>
@@ -2549,53 +3276,89 @@
       <c r="G37" s="1">
         <v>1</v>
       </c>
-      <c r="H37" s="13">
+      <c r="H37" s="11">
         <v>5.22</v>
       </c>
-      <c r="I37" s="13">
+      <c r="I37" s="11">
+        <f t="shared" si="1"/>
+        <v>5.22</v>
+      </c>
+      <c r="J37" s="17">
+        <f t="shared" si="2"/>
+        <v>6.5249999999999995</v>
+      </c>
+      <c r="K37" s="20">
+        <v>6</v>
+      </c>
+      <c r="L37" s="22">
+        <v>54</v>
+      </c>
+      <c r="M37" s="22">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N37" s="20">
         <f t="shared" si="0"/>
-        <v>5.22</v>
-      </c>
-      <c r="J37" s="13">
+        <v>6</v>
+      </c>
+      <c r="O37" s="16">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
+      </c>
+      <c r="H38" s="12">
+        <v>2.74</v>
+      </c>
+      <c r="I38" s="11">
         <f t="shared" si="1"/>
-        <v>6.5249999999999995</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="G38" s="11">
-        <v>1</v>
-      </c>
-      <c r="H38" s="14">
         <v>2.74</v>
       </c>
-      <c r="I38" s="13">
+      <c r="J38" s="17">
+        <f t="shared" si="2"/>
+        <v>3.4250000000000003</v>
+      </c>
+      <c r="K38" s="20">
+        <v>10</v>
+      </c>
+      <c r="L38" s="22">
+        <v>120</v>
+      </c>
+      <c r="M38" s="22">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N38" s="20">
         <f t="shared" si="0"/>
-        <v>2.74</v>
-      </c>
-      <c r="J38" s="13">
-        <f t="shared" si="1"/>
-        <v>3.4250000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O38" s="16">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -2617,53 +3380,89 @@
       <c r="G39" s="1">
         <v>1</v>
       </c>
-      <c r="H39" s="13">
+      <c r="H39" s="11">
         <v>2.71</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="11">
+        <f t="shared" si="1"/>
+        <v>2.71</v>
+      </c>
+      <c r="J39" s="17">
+        <f t="shared" si="2"/>
+        <v>3.3875000000000002</v>
+      </c>
+      <c r="K39" s="20">
+        <v>10</v>
+      </c>
+      <c r="L39" s="22">
+        <v>13</v>
+      </c>
+      <c r="M39" s="22">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
+      </c>
+      <c r="N39" s="20">
         <f t="shared" si="0"/>
-        <v>2.71</v>
-      </c>
-      <c r="J39" s="13">
+        <v>10</v>
+      </c>
+      <c r="O39" s="16">
+        <f t="shared" si="4"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40" s="10">
+        <v>1</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0.995</v>
+      </c>
+      <c r="I40" s="11">
         <f t="shared" si="1"/>
-        <v>3.3875000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G40" s="11">
-        <v>1</v>
-      </c>
-      <c r="H40" s="14">
         <v>0.995</v>
       </c>
-      <c r="I40" s="13">
+      <c r="J40" s="17">
+        <f t="shared" si="2"/>
+        <v>1.2437499999999999</v>
+      </c>
+      <c r="K40" s="20">
+        <v>5</v>
+      </c>
+      <c r="L40" s="22">
+        <v>22.25</v>
+      </c>
+      <c r="M40" s="22">
+        <f t="shared" si="3"/>
+        <v>4.45</v>
+      </c>
+      <c r="N40" s="20">
         <f t="shared" si="0"/>
-        <v>0.995</v>
-      </c>
-      <c r="J40" s="13">
-        <f t="shared" si="1"/>
-        <v>1.2437499999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="O40" s="16">
+        <f t="shared" si="4"/>
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -2685,53 +3484,89 @@
       <c r="G41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="13">
+      <c r="H41" s="11">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I41" s="13">
+      <c r="I41" s="11">
+        <f t="shared" si="1"/>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="J41" s="17">
+        <f t="shared" si="2"/>
+        <v>1.20875</v>
+      </c>
+      <c r="K41" s="20">
+        <v>5</v>
+      </c>
+      <c r="L41" s="22">
+        <v>30</v>
+      </c>
+      <c r="M41" s="22">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N41" s="20">
         <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J41" s="13">
+        <v>5</v>
+      </c>
+      <c r="O41" s="16">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="10">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="I42" s="11">
         <f t="shared" si="1"/>
-        <v>1.20875</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="11">
-        <v>1</v>
-      </c>
-      <c r="H42" s="14">
         <v>0.13</v>
       </c>
-      <c r="I42" s="13">
+      <c r="J42" s="17">
+        <f t="shared" si="2"/>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="K42" s="20">
+        <v>50</v>
+      </c>
+      <c r="L42" s="22">
+        <v>20</v>
+      </c>
+      <c r="M42" s="22">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="N42" s="20">
         <f t="shared" si="0"/>
-        <v>0.13</v>
-      </c>
-      <c r="J42" s="13">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="O42" s="16">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>182</v>
       </c>
@@ -2753,134 +3588,201 @@
       <c r="G43" s="1">
         <v>2</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H43" s="11">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="11">
+        <f t="shared" si="1"/>
+        <v>0.186</v>
+      </c>
+      <c r="J43" s="17">
+        <f t="shared" si="2"/>
+        <v>0.23249999999999998</v>
+      </c>
+      <c r="K43" s="20">
+        <v>0</v>
+      </c>
+      <c r="L43" s="22">
+        <v>0</v>
+      </c>
+      <c r="M43" s="22">
+        <v>0</v>
+      </c>
+      <c r="N43" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>0.186</v>
-      </c>
-      <c r="J43" s="13">
+        <v/>
+      </c>
+      <c r="O43" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" s="10">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12">
+        <v>1.26</v>
+      </c>
+      <c r="I44" s="11">
         <f t="shared" si="1"/>
-        <v>0.23249999999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G44" s="11">
-        <v>1</v>
-      </c>
-      <c r="H44" s="14">
         <v>1.26</v>
       </c>
-      <c r="I44" s="13">
+      <c r="J44" s="17">
+        <f t="shared" si="2"/>
+        <v>1.575</v>
+      </c>
+      <c r="K44" s="20">
+        <v>10</v>
+      </c>
+      <c r="L44" s="22">
+        <v>49</v>
+      </c>
+      <c r="M44" s="22">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N44" s="20">
         <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="J44" s="13">
-        <f t="shared" si="1"/>
-        <v>1.575</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O44" s="16">
+        <f t="shared" si="4"/>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="30">
         <v>691243110009</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="15">
         <v>691243110009</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="15">
         <v>691243110009</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>129</v>
       </c>
       <c r="G45" s="1">
-        <v>1</v>
-      </c>
-      <c r="H45" s="13">
+        <v>3</v>
+      </c>
+      <c r="H45" s="11">
         <v>3.7</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="11">
+        <f t="shared" si="1"/>
+        <v>11.100000000000001</v>
+      </c>
+      <c r="J45" s="17">
+        <f t="shared" si="2"/>
+        <v>13.875000000000002</v>
+      </c>
+      <c r="K45" s="20">
+        <v>50</v>
+      </c>
+      <c r="L45" s="22">
+        <v>23</v>
+      </c>
+      <c r="M45" s="22">
+        <f t="shared" si="3"/>
+        <v>0.46</v>
+      </c>
+      <c r="N45" s="20">
         <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="J45" s="13">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="O45" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="1">
+        <v>61300611821</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="10">
+        <v>61300611821</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="10">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I46" s="11">
         <f t="shared" si="1"/>
-        <v>4.625</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B46" s="11">
-        <v>61300611821</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="11">
-        <v>61300611821</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G46" s="11">
-        <v>1</v>
-      </c>
-      <c r="H46" s="14">
         <v>0.33500000000000002</v>
       </c>
-      <c r="I46" s="13">
+      <c r="J46" s="17">
+        <f t="shared" si="2"/>
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="K46" s="20">
+        <v>0</v>
+      </c>
+      <c r="L46" s="22">
+        <v>0</v>
+      </c>
+      <c r="M46" s="22">
+        <v>0</v>
+      </c>
+      <c r="N46" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="J46" s="13">
-        <f t="shared" si="1"/>
-        <v>0.41875000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="O46" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="15" t="s">
         <v>245</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E47" s="15" t="s">
         <v>244</v>
       </c>
       <c r="F47" s="1" t="s">
@@ -2889,94 +3791,126 @@
       <c r="G47" s="1">
         <v>1</v>
       </c>
-      <c r="H47" s="13">
+      <c r="H47" s="11">
         <v>0.59499999999999997</v>
       </c>
-      <c r="I47" s="13">
+      <c r="I47" s="11">
+        <f t="shared" si="1"/>
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="J47" s="17">
+        <f t="shared" si="2"/>
+        <v>0.74374999999999991</v>
+      </c>
+      <c r="K47" s="20">
+        <v>0</v>
+      </c>
+      <c r="L47" s="22">
+        <v>0</v>
+      </c>
+      <c r="M47" s="22">
+        <v>0</v>
+      </c>
+      <c r="N47" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="J47" s="13">
-        <f t="shared" si="1"/>
-        <v>0.74374999999999991</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="7" t="s">
+        <v/>
+      </c>
+      <c r="O47" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7">
         <f>SUM(J4:J47)</f>
-        <v>98.397500000000022</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+        <v>107.64750000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:15" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5" t="s">
         <v>140</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="8">
         <v>12.62</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="8">
         <f>F51*E51</f>
         <v>12.62</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="8">
         <f>G51*1.25</f>
         <v>15.774999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="K51" s="20">
+        <v>10</v>
+      </c>
+      <c r="L51" s="22">
+        <v>67</v>
+      </c>
+      <c r="M51" s="22">
+        <f t="shared" ref="M51" si="5">IF(K51&gt;0,L51/K51,"")</f>
+        <v>6.7</v>
+      </c>
+      <c r="O51" s="22">
+        <f>M51</f>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B52" s="10"/>
+      <c r="B52" s="9"/>
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52" s="8">
         <v>5.1100000000000003</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="8">
         <f>F52*E52</f>
         <v>5.1100000000000003</v>
       </c>
-      <c r="H52" s="9">
-        <f t="shared" ref="H52:H66" si="2">G52*1.25</f>
+      <c r="H52" s="8">
+        <f t="shared" ref="H52:H66" si="6">G52*1.25</f>
         <v>6.3875000000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M52" s="22"/>
+      <c r="O52" s="22"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>142</v>
       </c>
@@ -2984,19 +3918,21 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F53" s="8">
         <v>6.11</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="8">
         <f>F53*E53</f>
         <v>6.11</v>
       </c>
-      <c r="H53" s="9">
-        <f t="shared" si="2"/>
+      <c r="H53" s="8">
+        <f t="shared" si="6"/>
         <v>7.6375000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M53" s="22"/>
+      <c r="O53" s="22"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>211</v>
       </c>
@@ -3006,19 +3942,33 @@
       <c r="E54">
         <v>2</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54" s="8">
         <v>0.94899999999999995</v>
       </c>
-      <c r="G54" s="9">
-        <f t="shared" ref="G54:G66" si="3">F54*E54</f>
+      <c r="G54" s="8">
+        <f t="shared" ref="G54:G66" si="7">F54*E54</f>
         <v>1.8979999999999999</v>
       </c>
-      <c r="H54" s="9">
-        <f t="shared" si="2"/>
+      <c r="H54" s="8">
+        <f t="shared" si="6"/>
         <v>2.3725000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K54" s="19">
+        <v>10</v>
+      </c>
+      <c r="L54" s="19">
+        <v>16</v>
+      </c>
+      <c r="M54" s="22">
+        <f t="shared" ref="M54:M56" si="8">IF(K54&gt;0,L54/K54,"")</f>
+        <v>1.6</v>
+      </c>
+      <c r="O54" s="22">
+        <f>M54*2</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -3028,126 +3978,154 @@
       <c r="E55">
         <v>2</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55" s="8">
         <v>1.37</v>
       </c>
-      <c r="G55" s="9">
-        <f t="shared" si="3"/>
+      <c r="G55" s="8">
+        <f t="shared" si="7"/>
         <v>2.74</v>
       </c>
-      <c r="H55" s="9">
-        <f t="shared" si="2"/>
+      <c r="H55" s="8">
+        <f t="shared" si="6"/>
         <v>3.4250000000000003</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K55" s="19">
+        <v>10</v>
+      </c>
+      <c r="L55" s="19">
+        <v>16</v>
+      </c>
+      <c r="M55" s="22">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+      <c r="O55" s="22">
+        <f>M55*2</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>213</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="13" t="s">
         <v>208</v>
       </c>
       <c r="E56">
         <v>2</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F56" s="8">
         <v>0.84</v>
       </c>
-      <c r="G56" s="9">
-        <f t="shared" ref="G56" si="4">F56*E56</f>
+      <c r="G56" s="8">
+        <f t="shared" ref="G56" si="9">F56*E56</f>
         <v>1.68</v>
       </c>
-      <c r="H56" s="9">
-        <f t="shared" si="2"/>
+      <c r="H56" s="8">
+        <f t="shared" si="6"/>
         <v>2.1</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K56" s="19">
+        <v>10</v>
+      </c>
+      <c r="L56" s="19">
+        <v>16</v>
+      </c>
+      <c r="M56" s="22">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+      <c r="O56" s="22">
+        <f>M56*2</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="13" t="s">
         <v>197</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57" s="8">
         <v>0.875</v>
       </c>
-      <c r="G57" s="9">
-        <f t="shared" si="3"/>
+      <c r="G57" s="8">
+        <f t="shared" si="7"/>
         <v>0.875</v>
       </c>
-      <c r="H57" s="9">
-        <f t="shared" si="2"/>
+      <c r="H57" s="8">
+        <f t="shared" si="6"/>
         <v>1.09375</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>198</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="13" t="s">
         <v>199</v>
       </c>
       <c r="E58">
         <v>2</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58" s="8">
         <v>0.85599999999999998</v>
       </c>
-      <c r="G58" s="9">
-        <f t="shared" si="3"/>
+      <c r="G58" s="8">
+        <f t="shared" si="7"/>
         <v>1.712</v>
       </c>
-      <c r="H58" s="9">
-        <f t="shared" si="2"/>
+      <c r="H58" s="8">
+        <f t="shared" si="6"/>
         <v>2.14</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="13" t="s">
         <v>214</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="8">
         <v>3.45</v>
       </c>
-      <c r="G59" s="9">
-        <f t="shared" si="3"/>
+      <c r="G59" s="8">
+        <f t="shared" si="7"/>
         <v>3.45</v>
       </c>
-      <c r="H59" s="9">
-        <f t="shared" si="2"/>
+      <c r="H59" s="8">
+        <f t="shared" si="6"/>
         <v>4.3125</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>144</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F60" s="8">
         <v>5</v>
       </c>
-      <c r="G60" s="9">
-        <f t="shared" si="3"/>
+      <c r="G60" s="8">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="H60" s="9">
-        <f t="shared" si="2"/>
+      <c r="H60" s="8">
+        <f t="shared" si="6"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>203</v>
       </c>
@@ -3157,19 +4135,19 @@
       <c r="E61">
         <v>4</v>
       </c>
-      <c r="F61" s="9">
+      <c r="F61" s="8">
         <v>0.1</v>
       </c>
-      <c r="G61" s="9">
-        <f t="shared" si="3"/>
+      <c r="G61" s="8">
+        <f t="shared" si="7"/>
         <v>0.4</v>
       </c>
-      <c r="H61" s="9">
-        <f t="shared" si="2"/>
+      <c r="H61" s="8">
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>204</v>
       </c>
@@ -3179,20 +4157,20 @@
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" s="9">
+      <c r="F62" s="8">
         <v>0.1</v>
       </c>
-      <c r="G62" s="9">
-        <f t="shared" ref="G62" si="5">F62*E62</f>
+      <c r="G62" s="8">
+        <f t="shared" ref="G62" si="10">F62*E62</f>
         <v>0.1</v>
       </c>
-      <c r="H62" s="9">
-        <f t="shared" si="2"/>
+      <c r="H62" s="8">
+        <f t="shared" si="6"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>145</v>
       </c>
       <c r="B63" t="s">
@@ -3201,19 +4179,19 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" s="9">
+      <c r="F63" s="8">
         <v>0.2</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="8">
         <f>F61*E61</f>
         <v>0.4</v>
       </c>
-      <c r="H63" s="9">
-        <f t="shared" si="2"/>
+      <c r="H63" s="8">
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>206</v>
       </c>
@@ -3223,19 +4201,19 @@
       <c r="E64">
         <v>4</v>
       </c>
-      <c r="F64" s="9">
+      <c r="F64" s="8">
         <v>0.1</v>
       </c>
-      <c r="G64" s="9">
-        <f t="shared" si="3"/>
+      <c r="G64" s="8">
+        <f t="shared" si="7"/>
         <v>0.4</v>
       </c>
-      <c r="H64" s="9">
-        <f t="shared" si="2"/>
+      <c r="H64" s="8">
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>147</v>
       </c>
@@ -3245,19 +4223,19 @@
       <c r="E65">
         <v>2</v>
       </c>
-      <c r="F65" s="9">
+      <c r="F65" s="8">
         <v>0.1</v>
       </c>
-      <c r="G65" s="9">
-        <f t="shared" si="3"/>
+      <c r="G65" s="8">
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
-      <c r="H65" s="9">
-        <f t="shared" si="2"/>
+      <c r="H65" s="8">
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>248</v>
       </c>
@@ -3267,59 +4245,74 @@
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="F66" s="9">
-        <v>1</v>
-      </c>
-      <c r="G66" s="9">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H66" s="9">
-        <f t="shared" si="2"/>
+      <c r="F66" s="8">
+        <v>1</v>
+      </c>
+      <c r="G66" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H66" s="8">
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A67" s="7" t="s">
+    <row r="67" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7">
         <f>SUM(H64:H66)+SUM(H60:H62)+SUM(H53:H58)+H51</f>
         <v>43.418750000000003</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="18" t="s">
+      <c r="K67" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="L67" s="23">
+        <f>SUM(L4:L66)</f>
+        <v>1001.6800000000001</v>
+      </c>
+      <c r="N67" s="19">
+        <f>MIN(N4:N47)</f>
+        <v>2</v>
+      </c>
+      <c r="O67" s="16">
+        <f>SUM(O4:O66)</f>
+        <v>139.39119999999994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>150</v>
       </c>
       <c r="B70" t="s">
         <v>200</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="13" t="s">
         <v>227</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
-      <c r="F70" s="9">
+      <c r="F70" s="8">
         <v>171.4</v>
       </c>
-      <c r="G70" s="9">
-        <f t="shared" ref="G70" si="6">F70*E70</f>
+      <c r="G70" s="8">
+        <f t="shared" ref="G70" si="11">F70*E70</f>
         <v>171.4</v>
       </c>
       <c r="H70">
@@ -3327,55 +4320,55 @@
         <v>214.25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="18" t="s">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:15" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="13" t="s">
         <v>228</v>
       </c>
       <c r="E73">
         <v>1</v>
       </c>
-      <c r="F73" s="9">
+      <c r="F73" s="8">
         <v>17</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="8">
         <f>F73*E73</f>
         <v>17</v>
       </c>
-      <c r="H73" s="9">
+      <c r="H73" s="8">
         <f>G73*1.25</f>
         <v>21.25</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-    </row>
-    <row r="75" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="18" t="s">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+    </row>
+    <row r="75" spans="1:15" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="31"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>154</v>
       </c>
@@ -3385,19 +4378,19 @@
       <c r="E76">
         <v>1</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76" s="8">
         <v>66.34</v>
       </c>
-      <c r="G76" s="9">
-        <f t="shared" ref="G76:G77" si="7">F76*E76</f>
+      <c r="G76" s="8">
+        <f t="shared" ref="G76:G77" si="12">F76*E76</f>
         <v>66.34</v>
       </c>
-      <c r="H76" s="9">
-        <f t="shared" ref="H76:H81" si="8">G76*1.25</f>
+      <c r="H76" s="8">
+        <f t="shared" ref="H76:H81" si="13">G76*1.25</f>
         <v>82.925000000000011</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>230</v>
       </c>
@@ -3407,32 +4400,32 @@
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77" s="9">
+      <c r="F77" s="8">
         <v>38.340000000000003</v>
       </c>
-      <c r="G77" s="9">
-        <f t="shared" si="7"/>
+      <c r="G77" s="8">
+        <f t="shared" si="12"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H77" s="9">
-        <f t="shared" si="8"/>
+      <c r="H77" s="8">
+        <f t="shared" si="13"/>
         <v>47.925000000000004</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A78" s="7"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="9"/>
-    </row>
-    <row r="79" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="18" t="s">
+    <row r="78" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A78" s="6"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="8"/>
+    </row>
+    <row r="79" spans="1:15" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="H79" s="9"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="31"/>
+      <c r="H79" s="8"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>233</v>
       </c>
@@ -3442,15 +4435,15 @@
       <c r="E80">
         <v>1</v>
       </c>
-      <c r="F80" s="9">
+      <c r="F80" s="8">
         <v>18</v>
       </c>
-      <c r="G80" s="9">
-        <f t="shared" ref="G80:G81" si="9">F80*E80</f>
+      <c r="G80" s="8">
+        <f t="shared" ref="G80:G81" si="14">F80*E80</f>
         <v>18</v>
       </c>
-      <c r="H80" s="9">
-        <f t="shared" si="8"/>
+      <c r="H80" s="8">
+        <f t="shared" si="13"/>
         <v>22.5</v>
       </c>
     </row>
@@ -3464,15 +4457,15 @@
       <c r="E81">
         <v>1</v>
       </c>
-      <c r="F81" s="9">
+      <c r="F81" s="8">
         <v>17</v>
       </c>
-      <c r="G81" s="9">
-        <f t="shared" si="9"/>
+      <c r="G81" s="8">
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
-      <c r="H81" s="9">
-        <f t="shared" si="8"/>
+      <c r="H81" s="8">
+        <f t="shared" si="13"/>
         <v>21.25</v>
       </c>
     </row>
@@ -3490,6 +4483,59 @@
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C72:D72"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:B47">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>K4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M47">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M51:M56">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N47">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O51:O56">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D24" r:id="rId1" display="https://eu.mouser.com/manufacturer/cui-devices/" xr:uid="{20A6F0EA-5529-4B15-9D5D-90A5BC0CFECC}"/>
     <hyperlink ref="B57" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
@@ -3497,7 +4543,9 @@
     <hyperlink ref="B59" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
     <hyperlink ref="C70" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
     <hyperlink ref="B73" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
+    <hyperlink ref="B56" r:id="rId7" xr:uid="{1A1A304C-362E-44B6-95C3-66A5FDD7E9ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>